<commit_message>
SSDM-13256: Fixed failing tests.
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-type.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-type.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t xml:space="preserve">DATASET_TYPE</t>
   </si>
@@ -206,11 +206,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -227,14 +227,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -269,127 +269,115 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="F7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2" t="s">
+      <c r="G7" s="2"/>
+      <c r="H7" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
SSDM-13256: Fixed not correctly behaving compatible with import for vocabularies. Changed "Auto generate codes" to "Auto generate code" for samples.
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-type.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-type.xlsx
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t xml:space="preserve">DATASET_TYPE</t>
   </si>
   <si>
-    <t xml:space="preserve">Version</t>
-  </si>
-  <si>
     <t xml:space="preserve">Code</t>
   </si>
   <si>
@@ -35,9 +32,6 @@
   </si>
   <si>
     <t xml:space="preserve">Validation script</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
   </si>
   <si>
     <t xml:space="preserve">ATTACHMENT</t>
@@ -234,7 +228,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -254,127 +248,121 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="J6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>

</xml_diff>

<commit_message>
SSDM-13256: Added missing columns for data set types.
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-type.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-type.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t xml:space="preserve">DATASET_TYPE</t>
   </si>
@@ -34,12 +34,36 @@
     <t xml:space="preserve">Validation script</t>
   </si>
   <si>
+    <t xml:space="preserve">Main Data Set Pattern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main Data Set Path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disallow Deletion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modification Date</t>
+  </si>
+  <si>
     <t xml:space="preserve">ATTACHMENT</t>
   </si>
   <si>
     <t xml:space="preserve">Attachment</t>
   </si>
   <si>
+    <t xml:space="preserve">.*\.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">original/images/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FALSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-03-10 17:23:44</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mandatory</t>
   </si>
   <si>
@@ -65,9 +89,6 @@
   </si>
   <si>
     <t xml:space="preserve">$NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FALSE</t>
   </si>
   <si>
     <t xml:space="preserve">TRUE</t>
@@ -113,8 +134,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -195,7 +217,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -205,6 +227,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -228,7 +254,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -248,13 +274,37 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -262,107 +312,107 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="J6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>

</xml_diff>